<commit_message>
Updated Blink code, SCH comments & added LED mapping details
</commit_message>
<xml_diff>
--- a/Design/HLD_Design/Project_OAK_MCU_Pinouts.xlsx
+++ b/Design/HLD_Design/Project_OAK_MCU_Pinouts.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pin_Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="LED_Mapping" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="146">
   <si>
     <t>S. No</t>
   </si>
@@ -353,6 +354,105 @@
   </si>
   <si>
     <t>ANALOG POWER</t>
+  </si>
+  <si>
+    <t>Row Pin</t>
+  </si>
+  <si>
+    <t>Column Pin</t>
+  </si>
+  <si>
+    <t>LED Type</t>
+  </si>
+  <si>
+    <t>LED Value</t>
+  </si>
+  <si>
+    <t>WATCH DIAL LED Mapping</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PB2</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PD0</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>PD7</t>
+  </si>
+  <si>
+    <t>PE3</t>
   </si>
 </sst>
 </file>
@@ -383,7 +483,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,6 +553,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -658,6 +782,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,28 +878,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1057,8 +1202,8 @@
   <dimension ref="B2:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1079,17 +1224,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
       <c r="L2" s="2" t="s">
         <v>108</v>
       </c>
@@ -1098,25 +1243,25 @@
       </c>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="17" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="23" t="s">
         <v>103</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -1127,9 +1272,9 @@
       </c>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1142,8 +1287,8 @@
       <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
       <c r="L4" s="2" t="s">
         <v>110</v>
       </c>
@@ -1159,7 +1304,7 @@
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="43" t="s">
         <v>90</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -1186,7 +1331,7 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +1354,7 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1236,15 +1381,15 @@
       <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="6">
@@ -1253,13 +1398,13 @@
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="24"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="6">
@@ -1271,7 +1416,7 @@
       <c r="D10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="44" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -1281,10 +1426,10 @@
         <v>22</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="39" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1295,17 +1440,17 @@
       <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="34"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="40"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="6">
@@ -1314,15 +1459,15 @@
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="35"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="6">
@@ -1331,10 +1476,10 @@
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="44" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1356,8 +1501,8 @@
       <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1365,10 +1510,10 @@
         <v>31</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="19" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1379,15 +1524,15 @@
       <c r="C15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="14"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="6">
@@ -1396,8 +1541,8 @@
       <c r="C16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="6" t="s">
         <v>35</v>
       </c>
@@ -1405,8 +1550,8 @@
         <v>36</v>
       </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="14"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="6">
@@ -1415,15 +1560,15 @@
       <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="14"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="6">
@@ -1432,8 +1577,8 @@
       <c r="C18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="6" t="s">
         <v>40</v>
       </c>
@@ -1441,8 +1586,8 @@
         <v>45</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="15"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="6">
@@ -1451,8 +1596,8 @@
       <c r="C19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1462,10 +1607,10 @@
       <c r="H19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I19" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="38" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1476,8 +1621,8 @@
       <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="6" t="s">
         <v>47</v>
       </c>
@@ -1485,8 +1630,8 @@
         <v>48</v>
       </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="6">
@@ -1495,8 +1640,8 @@
       <c r="C21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="6" t="s">
         <v>50</v>
       </c>
@@ -1504,8 +1649,8 @@
         <v>51</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="32"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="38"/>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="6">
@@ -1514,15 +1659,15 @@
       <c r="C22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="6">
@@ -1531,19 +1676,19 @@
       <c r="C23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="15" t="s">
         <v>56</v>
       </c>
       <c r="I23" s="11" t="s">
@@ -1560,15 +1705,15 @@
       <c r="C24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="46"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="49"/>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="6">
@@ -1577,15 +1722,15 @@
       <c r="C25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="6">
@@ -1594,10 +1739,10 @@
       <c r="C26" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="43" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -1609,10 +1754,10 @@
       <c r="H26" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="19" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1623,8 +1768,8 @@
       <c r="C27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="6" t="s">
         <v>63</v>
       </c>
@@ -1632,8 +1777,8 @@
         <v>64</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="14"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="6">
@@ -1642,8 +1787,8 @@
       <c r="C28" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="6" t="s">
         <v>66</v>
       </c>
@@ -1651,8 +1796,8 @@
         <v>67</v>
       </c>
       <c r="H28" s="6"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="14"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="6">
@@ -1661,15 +1806,15 @@
       <c r="C29" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="14"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="6">
@@ -1678,15 +1823,15 @@
       <c r="C30" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="15"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="6">
@@ -1695,8 +1840,8 @@
       <c r="C31" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
       <c r="F31" s="6" t="s">
         <v>73</v>
       </c>
@@ -1704,10 +1849,10 @@
         <v>74</v>
       </c>
       <c r="H31" s="6"/>
-      <c r="I31" s="36" t="s">
+      <c r="I31" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="J31" s="31" t="s">
+      <c r="J31" s="37" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1718,8 +1863,8 @@
       <c r="C32" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="6" t="s">
         <v>76</v>
       </c>
@@ -1727,8 +1872,8 @@
         <v>77</v>
       </c>
       <c r="H32" s="6"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="31"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="37"/>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="6">
@@ -1737,15 +1882,15 @@
       <c r="C33" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="30"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1">
       <c r="B34" s="6">
@@ -1754,10 +1899,10 @@
       <c r="C34" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="37" t="s">
+      <c r="E34" s="43" t="s">
         <v>9</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -1767,10 +1912,10 @@
         <v>82</v>
       </c>
       <c r="H34" s="6"/>
-      <c r="I34" s="36" t="s">
+      <c r="I34" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="J34" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1781,8 +1926,8 @@
       <c r="C35" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
       <c r="F35" s="6" t="s">
         <v>84</v>
       </c>
@@ -1790,8 +1935,8 @@
         <v>85</v>
       </c>
       <c r="H35" s="6"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="16"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="6">
@@ -1800,8 +1945,8 @@
       <c r="C36" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="6" t="s">
         <v>87</v>
       </c>
@@ -1824,18 +1969,17 @@
     <mergeCell ref="D24:J24"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="E13:E21"/>
     <mergeCell ref="E26:E32"/>
     <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D11:D12"/>
     <mergeCell ref="D13:D21"/>
     <mergeCell ref="D26:D32"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="D3:D4"/>
     <mergeCell ref="J26:J30"/>
     <mergeCell ref="J34:J35"/>
     <mergeCell ref="J3:J4"/>
@@ -1851,6 +1995,915 @@
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="I26:I30"/>
     <mergeCell ref="I14:I18"/>
+    <mergeCell ref="I31:I32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H39"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="13">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="13">
+        <v>4</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="13">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="13">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="13">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="13">
+        <v>8</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="13">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="13">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="13">
+        <v>12</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="13">
+        <v>13</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="13">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="13">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="13">
+        <f>H17+2.5</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="13">
+        <v>16</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" s="13">
+        <f>H18+2.5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="13">
+        <v>17</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="13">
+        <f>H19+2.5</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="13">
+        <v>18</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="13">
+        <f>H20+2.5</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="13">
+        <v>19</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="13">
+        <v>20</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" s="13">
+        <f>H22-2.5</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="13">
+        <v>21</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H24" s="13">
+        <f>H23-2.5</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="13">
+        <v>22</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="13">
+        <f>H24-2.5</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="13">
+        <v>23</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H26" s="13">
+        <f>H25-2.5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="13">
+        <v>24</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="13">
+        <f>H26-2.5</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="13">
+        <v>25</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="13">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="13">
+        <v>26</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="13">
+        <f>H28+2.5</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="13">
+        <v>27</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H30" s="13">
+        <f>H29+2.5</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="13">
+        <v>28</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="13">
+        <f>H30+2.5</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="13">
+        <v>29</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" s="13">
+        <f>H31+2.5</f>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="13">
+        <v>30</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H33" s="13">
+        <f>H32+2.5</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="13">
+        <v>31</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="13">
+        <v>32</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35" s="13">
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="13">
+        <v>33</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="13">
+        <f>H35-2.5</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="13">
+        <v>34</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" s="13">
+        <f>H36-2.5</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="13">
+        <v>35</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" s="13">
+        <f>H37-2.5</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="13">
+        <v>36</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="13">
+        <f>H38-2.5</f>
+        <v>47.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>